<commit_message>
Se agrega tomar dias y horarios
</commit_message>
<xml_diff>
--- a/src/main/resources/Clases.xlsx
+++ b/src/main/resources/Clases.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandra/Documents/GitHub/ProgramacionDeVanguardia/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B6C0C6-9211-D34D-A8FF-71149448631D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44AC861D-C417-7144-9A4B-274BD14908AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="1" xr2:uid="{00C10C47-9D5E-A54D-9DA3-401045B4A976}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
-    <sheet name="Aerobox" sheetId="2" r:id="rId3"/>
+    <sheet name="Aerobox" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -133,10 +133,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -512,22 +511,20 @@
       <c r="D2" s="1">
         <v>0.75</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>10</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="2"/>
       <c r="H2" s="1">
         <v>0.75</v>
       </c>
-      <c r="I2" s="2">
-        <v>10</v>
-      </c>
-      <c r="K2" s="2"/>
+      <c r="I2">
+        <v>10</v>
+      </c>
       <c r="L2" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2">
         <v>10</v>
       </c>
       <c r="N2" t="s">
@@ -541,27 +538,25 @@
       <c r="B3" s="1">
         <v>0.375</v>
       </c>
-      <c r="C3" s="2">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2"/>
+      <c r="C3">
+        <v>10</v>
+      </c>
       <c r="F3" s="1">
         <v>0.375</v>
       </c>
-      <c r="G3" s="2">
-        <v>10</v>
-      </c>
-      <c r="I3" s="2"/>
+      <c r="G3">
+        <v>10</v>
+      </c>
       <c r="J3" s="1">
         <v>0.375</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3">
         <v>10</v>
       </c>
       <c r="L3" s="1">
         <v>0.375</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3">
         <v>10</v>
       </c>
       <c r="N3" t="s">
@@ -576,37 +571,37 @@
       <c r="B4" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>10</v>
       </c>
       <c r="D4" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>10</v>
       </c>
       <c r="F4" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>10</v>
       </c>
       <c r="H4" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4">
         <v>10</v>
       </c>
       <c r="J4" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4">
         <v>10</v>
       </c>
       <c r="L4" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4">
         <v>10</v>
       </c>
       <c r="N4" t="s">
@@ -621,32 +616,31 @@
       <c r="B5" s="1">
         <v>0.75</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>10</v>
       </c>
       <c r="D5" s="1">
         <v>0.375</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>10</v>
       </c>
       <c r="F5" s="1">
         <v>0.75</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>10</v>
       </c>
       <c r="H5" s="1">
         <v>0.375</v>
       </c>
-      <c r="I5" s="2">
-        <v>10</v>
-      </c>
-      <c r="K5" s="2"/>
+      <c r="I5">
+        <v>10</v>
+      </c>
       <c r="L5" s="1">
         <v>0.375</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5">
         <v>10</v>
       </c>
       <c r="N5" t="s">
@@ -661,27 +655,25 @@
       <c r="B6" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C6" s="2">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2"/>
+      <c r="C6">
+        <v>10</v>
+      </c>
       <c r="F6" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="G6" s="2">
-        <v>10</v>
-      </c>
-      <c r="I6" s="2"/>
+      <c r="G6">
+        <v>10</v>
+      </c>
       <c r="J6" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6">
         <v>10</v>
       </c>
       <c r="L6" s="1">
         <v>0.45833333333333331</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6">
         <v>10</v>
       </c>
       <c r="N6" t="s">
@@ -696,37 +688,37 @@
       <c r="B7" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>10</v>
       </c>
       <c r="D7" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <v>10</v>
       </c>
       <c r="F7" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7">
         <v>10</v>
       </c>
       <c r="H7" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7">
         <v>10</v>
       </c>
       <c r="J7" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7">
         <v>10</v>
       </c>
       <c r="L7" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7">
         <v>10</v>
       </c>
       <c r="N7" t="s">
@@ -741,37 +733,37 @@
       <c r="B8" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>10</v>
       </c>
       <c r="D8" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8">
         <v>10</v>
       </c>
       <c r="F8" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8">
         <v>10</v>
       </c>
       <c r="H8" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8">
         <v>10</v>
       </c>
       <c r="J8" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8">
         <v>10</v>
       </c>
       <c r="L8" s="1">
         <v>0.45833333333333331</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8">
         <v>10</v>
       </c>
       <c r="N8" t="s">
@@ -785,37 +777,37 @@
       <c r="B9" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>10</v>
       </c>
       <c r="D9" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9">
         <v>10</v>
       </c>
       <c r="F9" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9">
         <v>10</v>
       </c>
       <c r="H9" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9">
         <v>10</v>
       </c>
       <c r="J9" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9">
         <v>10</v>
       </c>
       <c r="L9" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9">
         <v>10</v>
       </c>
       <c r="N9" t="s">
@@ -831,23 +823,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0BE07DF-6E5B-634A-81C0-CE6FC25DF4B4}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0602F5DA-FE4D-AA46-B9B2-52B5F3996897}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -856,40 +836,52 @@
       <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4">
+      <c r="B1" s="3">
         <v>0.75</v>
       </c>
-      <c r="C1" s="3">
-        <v>10</v>
-      </c>
-      <c r="D1" s="3"/>
+      <c r="C1" s="2">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>0.75</v>
       </c>
-      <c r="C2" s="3">
-        <v>10</v>
-      </c>
-      <c r="D2" s="4"/>
+      <c r="C2" s="2">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C3" s="3">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3"/>
+      <c r="C3" s="2">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0BE07DF-6E5B-634A-81C0-CE6FC25DF4B4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega el logo
</commit_message>
<xml_diff>
--- a/src/main/resources/Clases.xlsx
+++ b/src/main/resources/Clases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandra/Documents/GitHub/ProgramacionDeVanguardia/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44AC861D-C417-7144-9A4B-274BD14908AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2521A9-2DE9-B34D-AEB5-4A5B621B9241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="1" xr2:uid="{00C10C47-9D5E-A54D-9DA3-401045B4A976}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Localizada</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>SABADO</t>
+  </si>
+  <si>
+    <t>"18:00"</t>
+  </si>
+  <si>
+    <t>"10:00"</t>
   </si>
 </sst>
 </file>
@@ -827,17 +833,20 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3">
-        <v>0.75</v>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C1" s="2">
         <v>10</v>
@@ -848,8 +857,8 @@
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.75</v>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="C2" s="2">
         <v>10</v>
@@ -860,8 +869,8 @@
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B3" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C3" s="2">
         <v>10</v>

</xml_diff>

<commit_message>
Se agregan dias y horarios
</commit_message>
<xml_diff>
--- a/src/main/resources/Clases.xlsx
+++ b/src/main/resources/Clases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandra/Documents/GitHub/ProgramacionDeVanguardia/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2521A9-2DE9-B34D-AEB5-4A5B621B9241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDB7C76-B605-8640-A905-EED1997ABAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="1" xr2:uid="{00C10C47-9D5E-A54D-9DA3-401045B4A976}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Localizada</t>
   </si>
@@ -92,12 +92,6 @@
   </si>
   <si>
     <t>SABADO</t>
-  </si>
-  <si>
-    <t>"18:00"</t>
-  </si>
-  <si>
-    <t>"10:00"</t>
   </si>
 </sst>
 </file>
@@ -833,7 +827,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,8 +839,8 @@
       <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>18</v>
+      <c r="B1" s="3">
+        <v>0.75</v>
       </c>
       <c r="C1" s="2">
         <v>10</v>
@@ -857,8 +851,8 @@
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>18</v>
+      <c r="B2" s="3">
+        <v>0.75</v>
       </c>
       <c r="C2" s="2">
         <v>10</v>
@@ -869,8 +863,8 @@
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>19</v>
+      <c r="B3" s="3">
+        <v>0.41666666666666669</v>
       </c>
       <c r="C3" s="2">
         <v>10</v>

</xml_diff>

<commit_message>
Se agrega que devuelva toda la clase
</commit_message>
<xml_diff>
--- a/src/main/resources/Clases.xlsx
+++ b/src/main/resources/Clases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandra/Documents/GitHub/ProgramacionDeVanguardia/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDB7C76-B605-8640-A905-EED1997ABAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5A1BA2-9D30-0D46-AB68-0435710D0AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="1" xr2:uid="{00C10C47-9D5E-A54D-9DA3-401045B4A976}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
   <si>
     <t>Localizada</t>
   </si>
@@ -459,7 +459,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -827,7 +827,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,7 +845,9 @@
       <c r="C1" s="2">
         <v>10</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -857,7 +859,9 @@
       <c r="C2" s="2">
         <v>10</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -869,7 +873,9 @@
       <c r="C3" s="2">
         <v>10</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Se resta el cupo de la clase anotada
</commit_message>
<xml_diff>
--- a/src/main/resources/Clases.xlsx
+++ b/src/main/resources/Clases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandra/Documents/GitHub/ProgramacionDeVanguardia/src/main/resources/"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -98,6 +98,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -464,46 +465,46 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="14" max="14" width="18.6640625" customWidth="1"/>
+    <col min="14" max="14" customWidth="true" width="18.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="F1" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>3</v>
       </c>
       <c r="B2" s="1"/>
@@ -511,306 +512,306 @@
       <c r="D2" s="1">
         <v>0.75</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>10</v>
       </c>
       <c r="F2" s="1"/>
       <c r="H2" s="1">
         <v>0.75</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="0">
         <v>10</v>
       </c>
       <c r="L2" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="M2">
-        <v>10</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="M2" s="0">
+        <v>10</v>
+      </c>
+      <c r="N2" t="s" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>0.375</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>10</v>
       </c>
       <c r="F3" s="1">
         <v>0.375</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>10</v>
       </c>
       <c r="J3" s="1">
         <v>0.375</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="0">
         <v>10</v>
       </c>
       <c r="L3" s="1">
         <v>0.375</v>
       </c>
-      <c r="M3">
-        <v>10</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="M3" s="0">
+        <v>10</v>
+      </c>
+      <c r="N3" t="s" s="0">
         <v>15</v>
       </c>
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <v>10</v>
       </c>
       <c r="D4" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <v>10</v>
       </c>
       <c r="F4" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>10</v>
       </c>
       <c r="H4" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="0">
         <v>10</v>
       </c>
       <c r="J4" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="0">
         <v>10</v>
       </c>
       <c r="L4" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="M4">
-        <v>10</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="M4" s="0">
+        <v>10</v>
+      </c>
+      <c r="N4" t="s" s="0">
         <v>14</v>
       </c>
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>0</v>
       </c>
       <c r="B5" s="1">
         <v>0.75</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0">
         <v>10</v>
       </c>
       <c r="D5" s="1">
         <v>0.375</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <v>10</v>
       </c>
       <c r="F5" s="1">
         <v>0.75</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>10</v>
       </c>
       <c r="H5" s="1">
         <v>0.375</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="0">
         <v>10</v>
       </c>
       <c r="L5" s="1">
         <v>0.375</v>
       </c>
-      <c r="M5">
-        <v>10</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="M5" s="0">
+        <v>10</v>
+      </c>
+      <c r="N5" t="s" s="0">
         <v>14</v>
       </c>
       <c r="O5" s="1"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0">
         <v>10</v>
       </c>
       <c r="F6" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <v>10</v>
       </c>
       <c r="J6" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="0">
         <v>10</v>
       </c>
       <c r="L6" s="1">
         <v>0.45833333333333331</v>
       </c>
-      <c r="M6">
-        <v>10</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="M6" s="0">
+        <v>10</v>
+      </c>
+      <c r="N6" t="s" s="0">
         <v>15</v>
       </c>
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>1</v>
       </c>
       <c r="B7" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="0">
         <v>10</v>
       </c>
       <c r="D7" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0">
         <v>10</v>
       </c>
       <c r="F7" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0">
         <v>10</v>
       </c>
       <c r="H7" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="0">
         <v>10</v>
       </c>
       <c r="J7" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="0">
         <v>10</v>
       </c>
       <c r="L7" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="M7">
-        <v>10</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="M7" s="0">
+        <v>10</v>
+      </c>
+      <c r="N7" t="s" s="0">
         <v>14</v>
       </c>
       <c r="O7" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="0">
         <v>10</v>
       </c>
       <c r="D8" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="0">
         <v>10</v>
       </c>
       <c r="F8" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <v>10</v>
       </c>
       <c r="H8" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="0">
         <v>10</v>
       </c>
       <c r="J8" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="0">
         <v>10</v>
       </c>
       <c r="L8" s="1">
         <v>0.45833333333333331</v>
       </c>
-      <c r="M8">
-        <v>10</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="M8" s="0">
+        <v>10</v>
+      </c>
+      <c r="N8" t="s" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>5</v>
       </c>
       <c r="B9" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="0">
         <v>10</v>
       </c>
       <c r="D9" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="0">
         <v>10</v>
       </c>
       <c r="F9" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="0">
         <v>10</v>
       </c>
       <c r="H9" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="0">
         <v>10</v>
       </c>
       <c r="J9" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="0">
         <v>10</v>
       </c>
       <c r="L9" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="M9">
-        <v>10</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="M9" s="0">
+        <v>10</v>
+      </c>
+      <c r="N9" t="s" s="0">
         <v>15</v>
       </c>
     </row>
@@ -832,11 +833,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>9</v>
       </c>
       <c r="B1" s="3">
@@ -845,7 +846,7 @@
       <c r="C1" s="2">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>15</v>
       </c>
     </row>
@@ -859,7 +860,7 @@
       <c r="C2" s="2">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>15</v>
       </c>
     </row>
@@ -870,10 +871,10 @@
       <c r="B3" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C3" s="2">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="2" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="D3" t="s" s="0">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mensaje de error si no hay mas cupo
</commit_message>
<xml_diff>
--- a/src/main/resources/Clases.xlsx
+++ b/src/main/resources/Clases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandra/Documents/GitHub/ProgramacionDeVanguardia/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5A1BA2-9D30-0D46-AB68-0435710D0AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E930D83A-E7C3-1043-A0BF-77443C4384F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="1" xr2:uid="{00C10C47-9D5E-A54D-9DA3-401045B4A976}"/>
   </bookViews>
@@ -828,7 +828,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -858,7 +858,7 @@
         <v>0.75</v>
       </c>
       <c r="C2" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>15</v>
@@ -872,7 +872,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>15</v>

</xml_diff>

<commit_message>
Se agregan las clases por entrenador
</commit_message>
<xml_diff>
--- a/src/main/resources/Clases.xlsx
+++ b/src/main/resources/Clases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandra/Documents/GitHub/ProgramacionDeVanguardia/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5B86CF-1EBA-224B-812F-FC94CF1B22DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7875A863-59DA-A94C-9C38-4D1310BB23F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="8" xr2:uid="{00C10C47-9D5E-A54D-9DA3-401045B4A976}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="1" xr2:uid="{00C10C47-9D5E-A54D-9DA3-401045B4A976}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -702,13 +702,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0602F5DA-FE4D-AA46-B9B2-52B5F3996897}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1061,7 +1064,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
@@ -1134,7 +1137,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -1292,7 +1295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83145F16-279F-3E4E-AFED-5BD5F6A2F7CD}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se agregan los alumnos al archivo
</commit_message>
<xml_diff>
--- a/src/main/resources/Clases.xlsx
+++ b/src/main/resources/Clases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandra/Documents/GitHub/ProgramacionDeVanguardia/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A25BA2A-AB23-B44D-802B-0327E08EF629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74ED4170-9670-BC4F-B3A1-EFAD217B6597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="1" xr2:uid="{00C10C47-9D5E-A54D-9DA3-401045B4A976}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="10" xr2:uid="{00C10C47-9D5E-A54D-9DA3-401045B4A976}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="Pesas" sheetId="7" r:id="rId7"/>
     <sheet name="Spinning" sheetId="8" r:id="rId8"/>
     <sheet name="Zumba" sheetId="9" r:id="rId9"/>
+    <sheet name="GIMENEZ ZAIRA" sheetId="10" r:id="rId10"/>
+    <sheet name="SANCHEZ ROBERTO" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -698,11 +700,37 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865722AA-ED35-D840-81B6-FC626094973F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB905C7-E257-BA4F-9987-8C6C869C6DBE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0602F5DA-FE4D-AA46-B9B2-52B5F3996897}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se guardan las clases reservadas
</commit_message>
<xml_diff>
--- a/src/main/resources/Clases.xlsx
+++ b/src/main/resources/Clases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandra/Documents/GitHub/ProgramacionDeVanguardia/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74ED4170-9670-BC4F-B3A1-EFAD217B6597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA849828-2886-EB41-B9CA-8742392FAE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="10" xr2:uid="{00C10C47-9D5E-A54D-9DA3-401045B4A976}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="22">
   <si>
     <t>Localizada</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>SÁBADO</t>
+  </si>
+  <si>
+    <t>LUNES 10:00</t>
+  </si>
+  <si>
+    <t>MARTES 08:00</t>
   </si>
 </sst>
 </file>
@@ -703,12 +709,29 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865722AA-ED35-D840-81B6-FC626094973F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -793,7 +816,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,7 +857,7 @@
         <v>0.375</v>
       </c>
       <c r="C3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>15</v>
@@ -904,8 +927,8 @@
       <c r="B3" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C3" t="n" s="0">
-        <v>1.0</v>
+      <c r="C3" s="0">
+        <v>1</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>14</v>
@@ -1032,8 +1055,8 @@
       <c r="B5" s="1">
         <v>0.375</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>1.0</v>
+      <c r="C5" s="0">
+        <v>1</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>14</v>
@@ -1061,8 +1084,8 @@
       <c r="B1" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C1" s="0">
-        <v>0</v>
+      <c r="C1" s="0" t="n">
+        <v>1.0</v>
       </c>
       <c r="D1" t="s" s="0">
         <v>15</v>
@@ -1248,8 +1271,8 @@
       <c r="B2" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C2" s="0">
-        <v>0</v>
+      <c r="C2" s="0" t="n">
+        <v>1.0</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>14</v>
@@ -1276,8 +1299,8 @@
       <c r="B4" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C4" s="0">
-        <v>0</v>
+      <c r="C4" t="n" s="0">
+        <v>1.0</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>14</v>
@@ -1390,8 +1413,8 @@
       <c r="B5" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C5" s="0">
-        <v>0</v>
+      <c r="C5" s="0" t="n">
+        <v>1.0</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>15</v>

</xml_diff>

<commit_message>
Se agrega para cancelar cupo
</commit_message>
<xml_diff>
--- a/src/main/resources/Clases.xlsx
+++ b/src/main/resources/Clases.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="23">
   <si>
     <t>Localizada</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>MARTES 08:00</t>
+  </si>
+  <si>
+    <t>MARTES 09:00</t>
   </si>
 </sst>
 </file>
@@ -709,7 +712,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865722AA-ED35-D840-81B6-FC626094973F}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -723,12 +726,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>21</v>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1013,8 +1016,8 @@
       <c r="B2" s="1">
         <v>0.375</v>
       </c>
-      <c r="C2" s="0">
-        <v>0</v>
+      <c r="C2" s="0" t="n">
+        <v>1.0</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>14</v>
@@ -1272,7 +1275,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>14</v>

</xml_diff>

<commit_message>
Revert "reservas de clases"
This reverts commit dc0e0f6a52648f6ea57c6bdfc7a619724c4cd8fd.
</commit_message>
<xml_diff>
--- a/src/main/resources/Clases.xlsx
+++ b/src/main/resources/Clases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandra/Documents/GitHub/ProgramacionDeVanguardia/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EF3503-AC27-DE4A-AD66-92A33124F86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA849828-2886-EB41-B9CA-8742392FAE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="5" xr2:uid="{00C10C47-9D5E-A54D-9DA3-401045B4A976}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="10" xr2:uid="{00C10C47-9D5E-A54D-9DA3-401045B4A976}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="23">
   <si>
     <t>Localizada</t>
   </si>
@@ -111,19 +111,10 @@
     <t>LUNES 10:00</t>
   </si>
   <si>
+    <t>MARTES 08:00</t>
+  </si>
+  <si>
     <t>MARTES 09:00</t>
-  </si>
-  <si>
-    <t>LUNES 08:00</t>
-  </si>
-  <si>
-    <t>MIÉRCOLES 08:00</t>
-  </si>
-  <si>
-    <t>MIÉRCOLES 18:00</t>
-  </si>
-  <si>
-    <t>VIERNES 10:00</t>
   </si>
 </sst>
 </file>
@@ -721,13 +712,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865722AA-ED35-D840-81B6-FC626094973F}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s" s="0">
         <v>6</v>
       </c>
@@ -735,36 +726,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s" s="0">
         <v>0</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -776,7 +743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB905C7-E257-BA4F-9987-8C6C869C6DBE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
@@ -791,7 +758,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -807,7 +774,7 @@
         <v>0.75</v>
       </c>
       <c r="C1" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s" s="0">
         <v>15</v>
@@ -821,7 +788,7 @@
         <v>0.75</v>
       </c>
       <c r="C2" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>15</v>
@@ -835,7 +802,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C3" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>15</v>
@@ -935,8 +902,8 @@
       <c r="B1" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C1" t="n" s="0">
-        <v>0.0</v>
+      <c r="C1" s="0">
+        <v>0</v>
       </c>
       <c r="D1" t="s" s="0">
         <v>14</v>
@@ -963,8 +930,8 @@
       <c r="B3" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>2.0</v>
+      <c r="C3" s="0">
+        <v>1</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>14</v>
@@ -1023,7 +990,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1049,8 +1016,8 @@
       <c r="B2" s="1">
         <v>0.375</v>
       </c>
-      <c r="C2" s="0">
-        <v>1</v>
+      <c r="C2" s="0" t="n">
+        <v>1.0</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>14</v>
@@ -1063,8 +1030,8 @@
       <c r="B3" s="1">
         <v>0.75</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>6.0</v>
+      <c r="C3" s="0">
+        <v>0</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>14</v>
@@ -1107,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F25638-7C88-2047-8D59-3EC4ECE34934}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1120,8 +1087,8 @@
       <c r="B1" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C1" s="0">
-        <v>1</v>
+      <c r="C1" s="0" t="n">
+        <v>1.0</v>
       </c>
       <c r="D1" t="s" s="0">
         <v>15</v>
@@ -1135,7 +1102,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C2" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>15</v>
@@ -1148,8 +1115,8 @@
       <c r="B3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>2.0</v>
+      <c r="C3" s="0">
+        <v>1</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>15</v>
@@ -1163,7 +1130,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="C4" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>15</v>
@@ -1307,8 +1274,8 @@
       <c r="B2" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C2" s="0">
-        <v>0</v>
+      <c r="C2" s="0" t="n">
+        <v>0.0</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>14</v>
@@ -1335,8 +1302,8 @@
       <c r="B4" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C4" s="0">
-        <v>1</v>
+      <c r="C4" t="n" s="0">
+        <v>1.0</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>14</v>
@@ -1449,8 +1416,8 @@
       <c r="B5" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C5" s="0">
-        <v>1</v>
+      <c r="C5" s="0" t="n">
+        <v>1.0</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>15</v>

</xml_diff>